<commit_message>
created list of pokemons to be included
</commit_message>
<xml_diff>
--- a/pokemon.xlsx
+++ b/pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\good6\Documents\GitHub\project-part-ii-wong-wan-ki-wong-keng-lam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B806AF8-D379-44D3-B07E-514D4D1F3593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E186FD-C6D6-4CB3-9BB6-A9E4DEFC0C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Pokemon</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +67,87 @@
   </si>
   <si>
     <t>dmg3</t>
+  </si>
+  <si>
+    <t>Bulbasaur</t>
+  </si>
+  <si>
+    <t>Seed Bomb</t>
+  </si>
+  <si>
+    <t>Sludge Bomb</t>
+  </si>
+  <si>
+    <t>Power Whip</t>
+  </si>
+  <si>
+    <t>Squirtle</t>
+  </si>
+  <si>
+    <t>Charmander</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Lapras</t>
+  </si>
+  <si>
+    <t>Snorlax</t>
+  </si>
+  <si>
+    <t>Mewtwo</t>
+  </si>
+  <si>
+    <t>Flamethrower</t>
+  </si>
+  <si>
+    <t>Flame Charge</t>
+  </si>
+  <si>
+    <t>Flame Burst</t>
+  </si>
+  <si>
+    <t>Discharge</t>
+  </si>
+  <si>
+    <t>Thunderbolt</t>
+  </si>
+  <si>
+    <t>Wild Charge</t>
+  </si>
+  <si>
+    <t>Aqua Jet</t>
+  </si>
+  <si>
+    <t>Aqua Tail</t>
+  </si>
+  <si>
+    <t>Water Pulse</t>
+  </si>
+  <si>
+    <t>Yawn</t>
+  </si>
+  <si>
+    <t>Hyper Beam</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>Frost Breath</t>
+  </si>
+  <si>
+    <t>Blizzazrd</t>
+  </si>
+  <si>
+    <t>Hydro Pump</t>
+  </si>
+  <si>
+    <t>Confusion</t>
+  </si>
+  <si>
+    <t>Ice Beam</t>
   </si>
 </sst>
 </file>
@@ -387,71 +465,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection sqref="A1:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>7.5</v>
+      </c>
+      <c r="D2">
+        <v>6.5</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>0.6</v>
+      </c>
+      <c r="G2">
+        <v>600</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>9.5</v>
+      </c>
+      <c r="D4">
+        <v>7.5</v>
+      </c>
+      <c r="E4">
+        <v>0.7</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>550</v>
+      </c>
+      <c r="H4">
+        <v>90</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>550</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6">
+        <v>480</v>
+      </c>
+      <c r="D6">
+        <v>450</v>
+      </c>
+      <c r="E6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6">
+        <v>1.9</v>
+      </c>
+      <c r="G6">
+        <v>1800</v>
+      </c>
+      <c r="H6">
+        <v>150</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6">
+        <v>40</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>240</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>2.8</v>
+      </c>
+      <c r="F7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G7">
+        <v>1400</v>
+      </c>
+      <c r="H7">
+        <v>150</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
+      <c r="C8">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>130</v>
+      </c>
+      <c r="E8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8">
+        <v>1.8</v>
+      </c>
+      <c r="G8">
+        <v>2200</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>